<commit_message>
potencia punta avlle llana
</commit_message>
<xml_diff>
--- a/archivos/ExcelResumenFactura.xlsx
+++ b/archivos/ExcelResumenFactura.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="89">
   <si>
     <t>archivo</t>
   </si>
@@ -112,6 +112,15 @@
     <t>13/03/2024</t>
   </si>
   <si>
+    <t>037</t>
+  </si>
+  <si>
+    <t>062</t>
+  </si>
+  <si>
+    <t>070</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -157,6 +166,15 @@
     <t>17.03.2024</t>
   </si>
   <si>
+    <t>29kWh</t>
+  </si>
+  <si>
+    <t>19kWh</t>
+  </si>
+  <si>
+    <t>39kWh</t>
+  </si>
+  <si>
     <t>67,79€</t>
   </si>
   <si>
@@ -191,6 +209,15 @@
   </si>
   <si>
     <t>01/10/2021</t>
+  </si>
+  <si>
+    <t>6 kWh</t>
+  </si>
+  <si>
+    <t>7 kWh</t>
+  </si>
+  <si>
+    <t>4 kWh</t>
   </si>
   <si>
     <t>1,43 €</t>
@@ -736,250 +763,253 @@
         <v>33</v>
       </c>
       <c r="L2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="N2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="O2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="P2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Q2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="R2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="S2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="T2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="U2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="V2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="W2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G3" t="s">
         <v>29</v>
       </c>
       <c r="H3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K3" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="L3" t="s">
-        <v>33</v>
+        <v>52</v>
+      </c>
+      <c r="M3" t="s">
+        <v>53</v>
       </c>
       <c r="N3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="O3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="P3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Q3" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="R3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="S3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="T3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="U3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="V3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="W3" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="G4" t="s">
         <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="I4" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="J4" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="K4" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="L4" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="M4" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="N4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="O4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="P4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Q4" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="R4" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="S4" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="T4" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="U4" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="V4" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="W4" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="E5" t="s">
         <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="G5" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="H5" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="I5" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="J5" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="K5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="L5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="M5" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="N5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="O5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="P5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Q5" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="R5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="S5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="T5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="U5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="V5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="W5" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>